<commit_message>
Periodo de pago en asignaciones
Nuevo campo para periodo de pago en asignaciones
</commit_message>
<xml_diff>
--- a/location/l10n_sv_hr_asignaciones/static/src/plantilla/plantilla_asignaciones.xlsx
+++ b/location/l10n_sv_hr_asignaciones/static/src/plantilla/plantilla_asignaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INCOE\Documents\GitHub\fe\location\l10n_sv_hr_asignaciones\static\src\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0891ED14-506A-4073-A9B6-EF1200EC7780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79517011-E1F1-48B0-A80D-F5E27E3FA4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1065" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guía" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>Descripción</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>Importante:</t>
+  </si>
+  <si>
+    <t>periodo_pago</t>
+  </si>
+  <si>
+    <t>Fecha efectiva (día real de la asignacion)</t>
+  </si>
+  <si>
+    <t>Fecha de corte/quincena que paga la asignación</t>
   </si>
 </sst>
 </file>
@@ -180,12 +189,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -557,57 +575,73 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>4</v>
+        <v>34</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>13</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>14</v>
       </c>
     </row>
@@ -618,10 +652,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,15 +663,16 @@
     <col min="1" max="1" width="16.88671875" customWidth="1"/>
     <col min="2" max="2" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.88671875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -647,35 +682,30 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -702,10 +732,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB4BDFD-FBAC-4B96-836E-5AF86AA041A1}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,11 +743,12 @@
     <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.109375" customWidth="1"/>
     <col min="3" max="3" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -727,18 +758,21 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modificación en plantilla de asignaciones
</commit_message>
<xml_diff>
--- a/location/l10n_sv_hr_asignaciones/static/src/plantilla/plantilla_asignaciones.xlsx
+++ b/location/l10n_sv_hr_asignaciones/static/src/plantilla/plantilla_asignaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INCOE\Documents\GitHub\fe\location\l10n_sv_hr_asignaciones\static\src\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79517011-E1F1-48B0-A80D-F5E27E3FA4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48710659-5156-400D-9AAA-9C02F510F272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guía" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Descripción</t>
   </si>
@@ -137,15 +137,6 @@
   </si>
   <si>
     <t>Importante:</t>
-  </si>
-  <si>
-    <t>periodo_pago</t>
-  </si>
-  <si>
-    <t>Fecha efectiva (día real de la asignacion)</t>
-  </si>
-  <si>
-    <t>Fecha de corte/quincena que paga la asignación</t>
   </si>
 </sst>
 </file>
@@ -189,18 +180,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -506,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -575,73 +560,57 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>35</v>
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>36</v>
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" t="s">
         <v>14</v>
       </c>
     </row>
@@ -652,10 +621,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,16 +632,15 @@
     <col min="1" max="1" width="16.88671875" customWidth="1"/>
     <col min="2" max="2" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.88671875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -683,27 +651,24 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -732,10 +697,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB4BDFD-FBAC-4B96-836E-5AF86AA041A1}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,12 +708,11 @@
     <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.109375" customWidth="1"/>
     <col min="3" max="3" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -758,21 +722,18 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>34</v>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
nueva tabla horas extras
</commit_message>
<xml_diff>
--- a/location/l10n_sv_hr_asignaciones/static/src/plantilla/plantilla_asignaciones.xlsx
+++ b/location/l10n_sv_hr_asignaciones/static/src/plantilla/plantilla_asignaciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INCOE\Documents\GitHub\fe\location\l10n_sv_hr_asignaciones\static\src\plantilla\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\fe\location\l10n_sv_hr_asignaciones\static\src\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48710659-5156-400D-9AAA-9C02F510F272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F1D876-3B8B-4734-B038-08723AA64FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guía" sheetId="2" r:id="rId1"/>
@@ -19,23 +19,11 @@
     <sheet name="OpcionesTipo" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Descripción</t>
   </si>
@@ -52,9 +40,6 @@
     <t>Cantidad de horas extra diurnas</t>
   </si>
   <si>
-    <t>horas_nocturnas</t>
-  </si>
-  <si>
     <t>Cantidad de horas extra nocturnas</t>
   </si>
   <si>
@@ -137,6 +122,24 @@
   </si>
   <si>
     <t>Importante:</t>
+  </si>
+  <si>
+    <t>horas_extras/horas_diurnas</t>
+  </si>
+  <si>
+    <t>horas_extras/horas_nocturnas</t>
+  </si>
+  <si>
+    <t>horas_extras/horas_diurnas_descanso</t>
+  </si>
+  <si>
+    <t>horas_extras/horas_nocturnas_descanso</t>
+  </si>
+  <si>
+    <t>horas_extras/horas_diurnas_asueto</t>
+  </si>
+  <si>
+    <t>horas_extras/horas_nocturnas_asueto</t>
   </si>
 </sst>
 </file>
@@ -493,80 +496,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="77.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>30</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -574,44 +577,44 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>9</v>
       </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>11</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>13</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -623,50 +626,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" customWidth="1"/>
+    <col min="2" max="2" width="4.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.53125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -703,27 +707,27 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1328125" customWidth="1"/>
+    <col min="3" max="3" width="7.796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -766,34 +770,34 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NO BAJAR CODIGO. nomina mensual y correccion de iva en planilla de facturas
</commit_message>
<xml_diff>
--- a/location/l10n_sv_hr_asignaciones/static/src/plantilla/plantilla_asignaciones.xlsx
+++ b/location/l10n_sv_hr_asignaciones/static/src/plantilla/plantilla_asignaciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\fe\location\l10n_sv_hr_asignaciones\static\src\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F1D876-3B8B-4734-B038-08723AA64FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB3DFE3-ABE0-4AD0-92F1-BD7CDC8E3B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guía" sheetId="2" r:id="rId1"/>
@@ -500,60 +500,60 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="77.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -561,7 +561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -569,7 +569,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -577,7 +577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -585,7 +585,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -593,7 +593,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -601,7 +601,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -609,7 +609,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -626,25 +626,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.86328125" customWidth="1"/>
-    <col min="2" max="2" width="4.53125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.84375" customWidth="1"/>
+    <col min="2" max="2" width="13.23046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.07421875" customWidth="1"/>
+    <col min="4" max="4" width="24.61328125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.53125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.73046875" customWidth="1"/>
+    <col min="6" max="6" width="33.69140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.53515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -707,16 +707,16 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1328125" customWidth="1"/>
-    <col min="3" max="3" width="7.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.15234375" customWidth="1"/>
+    <col min="3" max="3" width="7.765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.69140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -770,32 +770,32 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Correccion para nomina con multiples empresas
</commit_message>
<xml_diff>
--- a/location/l10n_sv_hr_asignaciones/static/src/plantilla/plantilla_asignaciones.xlsx
+++ b/location/l10n_sv_hr_asignaciones/static/src/plantilla/plantilla_asignaciones.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\fe\location\l10n_sv_hr_asignaciones\static\src\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB3DFE3-ABE0-4AD0-92F1-BD7CDC8E3B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681055E5-4A3A-428F-9288-76E3BDD06186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guía" sheetId="2" r:id="rId1"/>
     <sheet name="Horas Extra" sheetId="1" r:id="rId2"/>
     <sheet name="Asignaciones" sheetId="4" r:id="rId3"/>
     <sheet name="OpcionesTipo" sheetId="3" r:id="rId4"/>
+    <sheet name="Empresas" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>Descripción</t>
   </si>
@@ -140,6 +141,18 @@
   </si>
   <si>
     <t>horas_extras/horas_nocturnas_asueto</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>AE DE PAZ</t>
+  </si>
+  <si>
+    <t>INNUFFE</t>
+  </si>
+  <si>
+    <t>INVERSIONES COMERCIALES ESCOBAR SA DE CV</t>
   </si>
 </sst>
 </file>
@@ -171,7 +184,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -179,11 +192,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -191,6 +243,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -626,7 +684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -701,60 +759,69 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB4BDFD-FBAC-4B96-836E-5AF86AA041A1}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="16.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.15234375" customWidth="1"/>
-    <col min="3" max="3" width="7.765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.69140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.4609375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.61328125" customWidth="1"/>
+    <col min="4" max="4" width="14.4609375" customWidth="1"/>
+    <col min="5" max="5" width="12.07421875" customWidth="1"/>
+    <col min="6" max="6" width="22.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9BFC39DE-0A78-46B1-B0BE-EC5C226DD98F}">
           <x14:formula1>
             <xm:f>OpcionesTipo!$A$3:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B1048576</xm:sqref>
+          <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BE7FE6C6-2B0D-4C6B-855D-B18CBC410611}">
           <x14:formula1>
             <xm:f>Guía!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>B1</xm:sqref>
+          <xm:sqref>C1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AF84B292-0F28-4E84-B9C8-B0E3C1C27251}">
+          <x14:formula1>
+            <xm:f>Empresas!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -767,7 +834,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -804,4 +871,42 @@
   <sheetProtection algorithmName="SHA-512" hashValue="kpnTmtWGxoWSJz8BSuNTj4GgSVAXOkcWPjlpyYjRF+UUFcJbDpcHmGb6Fk4ovk8fkNqX17QEFzUu237TDh8t9Q==" saltValue="LIBin5KXRuqB3fjPpTUK1g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EFC7256-9EB7-448B-9811-D431BB963277}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="40.4609375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A3" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A4" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>